<commit_message>
added chart for introductory 3D
</commit_message>
<xml_diff>
--- a/visualisation/selected_courses.xlsx
+++ b/visualisation/selected_courses.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="73">
   <si>
     <t>Design of User Interfaces and Data</t>
   </si>
@@ -163,6 +163,81 @@
   </si>
   <si>
     <t>line_of_studies</t>
+  </si>
+  <si>
+    <t>Introductory 3D</t>
+  </si>
+  <si>
+    <t>KDDK</t>
+  </si>
+  <si>
+    <t>['Lise Jensen']</t>
+  </si>
+  <si>
+    <t>[{'room': 'Multimedielab', 'type': 'Forel√¶sning', 'day': 'Tirsdag', 'time_slot': '09.00-12.00'}]</t>
+  </si>
+  <si>
+    <t>cand.it. digital design og kommunikation (ddk)</t>
+  </si>
+  <si>
+    <t>['Anette Kreutzberg']</t>
+  </si>
+  <si>
+    <t>[{'room': 'Multimedielab', 'type': 'Forel√¶sning', 'day': 'Mandag', 'time_slot': '10.00-12.00'}, {'room': 'Multimedielab', 'type': '√òvelser', 'day': 'Mandag', 'time_slot': '13.00-15.00'}]</t>
+  </si>
+  <si>
+    <t>[{'room': None, 'type': 'Forel√¶sning', 'day': 'Mandag', 'time_slot': '10.00-12.00'}, {'room': None, 'type': '√òvelser', 'day': 'Mandag', 'time_slot': '13.00-15.00'}]</t>
+  </si>
+  <si>
+    <t>[{'room': 'Multimedielab', 'type': 'Forel√¶sning', 'day': 'Mandag', 'time_slot': '17.00-19.00'}, {'room': 'Multimedielab', 'type': '√òvelser', 'day': 'Mandag', 'time_slot': '19.00-21.00'}]</t>
+  </si>
+  <si>
+    <t>['KyoungHee Oh Holmen']</t>
+  </si>
+  <si>
+    <t>2009b</t>
+  </si>
+  <si>
+    <t>[{'room': '3A52 - teaching from 12:30-16:30', 'type': 'Forel√¶sning', 'day': 'Mandag', 'time_slot': '13.00-16.00'}, {'room': '3A52 - teaching from 12:30-16:30', 'type': '√òvelser', 'day': 'Mandag', 'time_slot': '13.00-16.00'}]</t>
+  </si>
+  <si>
+    <t>[{'room': '4A56', 'type': 'Forel√¶sning', 'day': 'Torsdag', 'time_slot': '13.45-15.45'}, {'room': '4A56', 'type': '√òvelser', 'day': 'Torsdag', 'time_slot': '16.00-18.00'}]</t>
+  </si>
+  <si>
+    <t>['Rickard Stampe S√∂derstr√∂m']</t>
+  </si>
+  <si>
+    <t>[{'room': 'GameLab', 'type': 'Forel√¶sning', 'day': 'Mandag', 'time_slot': '17.00-18.50'}, {'room': 'GameLab', 'type': '√òvelser', 'day': 'Mandag', 'time_slot': '19.00-20.50'}]</t>
+  </si>
+  <si>
+    <t>2012b</t>
+  </si>
+  <si>
+    <t>[{'room': 'GameLab ', 'type': 'Forel√¶sning', 'day': 'Mandag', 'time_slot': '17.00-18.50'}, {'room': 'GameLab ', 'type': '√òvelser', 'day': 'Mandag', 'time_slot': '19.00-20.50'}]</t>
+  </si>
+  <si>
+    <t>2013a</t>
+  </si>
+  <si>
+    <t>[{'room': '5A12/16', 'type': 'Forel√¶sning', 'day': 'Tirsdag', 'time_slot': '17.00-18.50'}, {'room': '5A12/12', 'type': '√òvelser', 'day': 'Tirsdag', 'time_slot': '19.00-20.50'}]</t>
+  </si>
+  <si>
+    <t>2013b</t>
+  </si>
+  <si>
+    <t>[{'room': '3A52PC', 'type': 'Forel√¶sning', 'day': 'Mandag', 'time_slot': '17.00-18.50'}, {'room': '3A52PC', 'type': '√òvelser', 'day': 'Mandag', 'time_slot': '19.00-20.50'}]</t>
+  </si>
+  <si>
+    <t>2014a</t>
+  </si>
+  <si>
+    <t>[{'room': '3A52', 'type': '√òvelser', 'day': 'Tirsdag', 'time_slot': '17.00-18.50'}, {'room': '3A52', 'type': 'Forel√¶sning', 'day': 'Tirsdag', 'time_slot': '19.00-20.50'}]</t>
+  </si>
+  <si>
+    <t>['KyoungHee Oh Holmen'] + ['Lise Jensen']</t>
+  </si>
+  <si>
+    <t>['Anette Kreutzberg'] + ['Lise Jensen']</t>
   </si>
 </sst>
 </file>
@@ -219,8 +294,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -230,9 +307,11 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -630,6 +709,432 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>overall_evaluation</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$40:$C$52</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2006b</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2007a</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2007b</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2008a</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2008b</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2009a</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2009b</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2010b</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2011b</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2012b</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2013a</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2013b</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2014a</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$40:$D$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.91</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.86</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.43</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.17</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.43</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>time_evaluation</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$40:$C$52</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2006b</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2007a</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2007b</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2008a</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2008b</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2009a</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2009b</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2010b</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2011b</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2012b</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2013a</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2013b</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2014a</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$40:$E$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.71</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.08</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.89</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.62</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.08</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.71</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>job_evaluation</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$40:$C$52</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2006b</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2007a</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2007b</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2008a</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2008b</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2009a</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2009b</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2010b</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2011b</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2012b</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2013a</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2013b</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2014a</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$40:$F$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>4.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.55</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.71</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.69</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.57</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.33</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.29</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.58</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.17</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.71</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2135018104"/>
+        <c:axId val="2128917176"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2135018104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2128917176"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2128917176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2135018104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -657,6 +1162,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1574800</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>43180</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -987,16 +1522,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="50.5" customWidth="1"/>
-    <col min="8" max="8" width="137" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" customWidth="1"/>
+    <col min="7" max="7" width="26.1640625" customWidth="1"/>
+    <col min="8" max="8" width="144.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="3" customFormat="1">
@@ -1597,6 +2133,706 @@
       </c>
       <c r="P12" s="1" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" s="3" customFormat="1">
+      <c r="A39" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L39" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M39" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="N39" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O39" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P39" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
+      <c r="A40" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40">
+        <v>5.4</v>
+      </c>
+      <c r="E40">
+        <v>3.6</v>
+      </c>
+      <c r="F40">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>35</v>
+      </c>
+      <c r="L40">
+        <v>0.2</v>
+      </c>
+      <c r="M40">
+        <v>35</v>
+      </c>
+      <c r="N40">
+        <v>750</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
+      <c r="A41" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41">
+        <v>5.91</v>
+      </c>
+      <c r="E41">
+        <v>4</v>
+      </c>
+      <c r="F41">
+        <v>5.55</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J41">
+        <v>12</v>
+      </c>
+      <c r="K41">
+        <v>35</v>
+      </c>
+      <c r="L41">
+        <v>0.32352941176470501</v>
+      </c>
+      <c r="M41">
+        <v>35</v>
+      </c>
+      <c r="N41">
+        <v>750</v>
+      </c>
+      <c r="O41" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
+      <c r="A42" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42">
+        <v>6</v>
+      </c>
+      <c r="E42">
+        <v>4.71</v>
+      </c>
+      <c r="F42">
+        <v>3.71</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J42">
+        <v>12</v>
+      </c>
+      <c r="K42">
+        <v>35</v>
+      </c>
+      <c r="L42">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="M42">
+        <v>35</v>
+      </c>
+      <c r="N42">
+        <v>750</v>
+      </c>
+      <c r="O42" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P42" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
+      <c r="A43" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43">
+        <v>5.46</v>
+      </c>
+      <c r="E43">
+        <v>4.08</v>
+      </c>
+      <c r="F43">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J43">
+        <v>12</v>
+      </c>
+      <c r="K43">
+        <v>35</v>
+      </c>
+      <c r="L43">
+        <v>0.40625</v>
+      </c>
+      <c r="M43">
+        <v>35</v>
+      </c>
+      <c r="N43">
+        <v>750</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
+      <c r="A44" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44">
+        <v>2.86</v>
+      </c>
+      <c r="E44">
+        <v>5</v>
+      </c>
+      <c r="F44">
+        <v>3.57</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J44">
+        <v>12</v>
+      </c>
+      <c r="K44">
+        <v>35</v>
+      </c>
+      <c r="L44">
+        <v>0.36842105263157798</v>
+      </c>
+      <c r="M44">
+        <v>35</v>
+      </c>
+      <c r="N44">
+        <v>750</v>
+      </c>
+      <c r="O44" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P44" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
+      <c r="A45" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D45">
+        <v>5</v>
+      </c>
+      <c r="E45">
+        <v>2.89</v>
+      </c>
+      <c r="F45">
+        <v>4.33</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J45">
+        <v>12</v>
+      </c>
+      <c r="K45">
+        <v>35</v>
+      </c>
+      <c r="L45">
+        <v>0.24324324324324301</v>
+      </c>
+      <c r="M45">
+        <v>35</v>
+      </c>
+      <c r="N45">
+        <v>750</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P45" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
+      <c r="A46" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D46">
+        <v>3</v>
+      </c>
+      <c r="E46">
+        <v>4</v>
+      </c>
+      <c r="F46">
+        <v>2</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J46">
+        <v>12</v>
+      </c>
+      <c r="K46">
+        <v>35</v>
+      </c>
+      <c r="L46">
+        <v>0.2</v>
+      </c>
+      <c r="M46">
+        <v>35</v>
+      </c>
+      <c r="N46">
+        <v>750</v>
+      </c>
+      <c r="O46" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P46" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="A47" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D47">
+        <v>4.43</v>
+      </c>
+      <c r="E47">
+        <v>4</v>
+      </c>
+      <c r="F47">
+        <v>4.29</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J47">
+        <v>12</v>
+      </c>
+      <c r="K47">
+        <v>35</v>
+      </c>
+      <c r="L47">
+        <v>0.53846153846153799</v>
+      </c>
+      <c r="M47">
+        <v>35</v>
+      </c>
+      <c r="N47">
+        <v>750</v>
+      </c>
+      <c r="O47" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P47" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
+      <c r="A48" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D48">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="E48">
+        <v>4.62</v>
+      </c>
+      <c r="F48">
+        <v>4.25</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J48">
+        <v>12</v>
+      </c>
+      <c r="K48">
+        <v>35</v>
+      </c>
+      <c r="L48">
+        <v>0.52941176470588203</v>
+      </c>
+      <c r="M48">
+        <v>35</v>
+      </c>
+      <c r="N48">
+        <v>750</v>
+      </c>
+      <c r="O48" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P48" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16">
+      <c r="A49" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49">
+        <v>5.25</v>
+      </c>
+      <c r="E49">
+        <v>4.08</v>
+      </c>
+      <c r="F49">
+        <v>4.58</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J49">
+        <v>12</v>
+      </c>
+      <c r="K49">
+        <v>35</v>
+      </c>
+      <c r="L49">
+        <v>0.35294117647058798</v>
+      </c>
+      <c r="M49">
+        <v>35</v>
+      </c>
+      <c r="N49">
+        <v>750</v>
+      </c>
+      <c r="O49" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P49" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16">
+      <c r="A50" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D50">
+        <v>5.17</v>
+      </c>
+      <c r="E50">
+        <v>3.25</v>
+      </c>
+      <c r="F50">
+        <v>4.17</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J50">
+        <v>12</v>
+      </c>
+      <c r="K50">
+        <v>35</v>
+      </c>
+      <c r="L50">
+        <v>0.28571428571428498</v>
+      </c>
+      <c r="M50">
+        <v>35</v>
+      </c>
+      <c r="N50">
+        <v>750</v>
+      </c>
+      <c r="O50" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P50" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16">
+      <c r="A51" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D51">
+        <v>5.43</v>
+      </c>
+      <c r="E51">
+        <v>3.71</v>
+      </c>
+      <c r="F51">
+        <v>4.71</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J51">
+        <v>12</v>
+      </c>
+      <c r="K51">
+        <v>35</v>
+      </c>
+      <c r="L51">
+        <v>0.233333333333333</v>
+      </c>
+      <c r="M51">
+        <v>35</v>
+      </c>
+      <c r="N51">
+        <v>750</v>
+      </c>
+      <c r="O51" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P51" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16">
+      <c r="A52" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D52">
+        <v>5.3</v>
+      </c>
+      <c r="E52">
+        <v>3.9</v>
+      </c>
+      <c r="F52">
+        <v>4.3</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J52">
+        <v>12</v>
+      </c>
+      <c r="K52">
+        <v>35</v>
+      </c>
+      <c r="L52">
+        <v>0.45454545454545398</v>
+      </c>
+      <c r="M52">
+        <v>35</v>
+      </c>
+      <c r="N52">
+        <v>750</v>
+      </c>
+      <c r="O52" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P52" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>